<commit_message>
Clean up admin work + meeting tracking
</commit_message>
<xml_diff>
--- a/Stage 4/Evidence/Meeting Tracking.xlsx
+++ b/Stage 4/Evidence/Meeting Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samli\Documents\Yuconz\27a\Stage 3\Evidence\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samli\Documents\Yuconz\27a\Stage 4\Evidence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607B2991-CF92-4B7F-AFB0-3CFDE74F0B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862C8DE6-08A4-4323-B7C7-E72838987F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E293897E-8EBF-4E9F-923A-8549BB33F108}"/>
+    <workbookView xWindow="4680" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{E293897E-8EBF-4E9F-923A-8549BB33F108}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -723,7 +723,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2430,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44F4C73-AD10-409F-A536-9F4A3BF21FD4}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2493,7 +2493,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -2565,7 +2565,7 @@
         <v>7.5</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>